<commit_message>
Update README.md and add some literature on MPPT
</commit_message>
<xml_diff>
--- a/BQ25570_Design_Help_V1_3.xlsx
+++ b/BQ25570_Design_Help_V1_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbe\Documents\eagle\repos\EHM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2125,7 +2125,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O22" sqref="O22"/>
+      <selection pane="topRight" activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2320,7 +2320,7 @@
         <v>34</v>
       </c>
       <c r="U7" s="13">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>58</v>
@@ -2413,7 +2413,7 @@
         <v>44</v>
       </c>
       <c r="O9" s="13">
-        <v>2.65</v>
+        <v>2.7</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>1</v>
@@ -2569,15 +2569,15 @@
       </c>
       <c r="U13" s="31">
         <f>IF(U9/U8*U7&gt;10, U9/U8*U7-10, U9/U8*U7)</f>
-        <v>8</v>
+        <v>5.2</v>
       </c>
       <c r="V13" s="52">
         <f>IF(U13&gt;1,VLOOKUP(U13*10,$AA$27:$AA$133,1)/10,IF(U13&gt;0.099,VLOOKUP(U13*100,$AB$27:$AB$133,1)/100,VLOOKUP(U13*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>7.87</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="W13" s="52">
         <f ca="1">IF(U13&gt;1,OFFSET($AA$27,MATCH(U13*10,$AA$27:$AA$133,1),0)/10,IF(U13&gt;0.099, OFFSET($AB$27,MATCH(U13*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(U13*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>8.0599999999999987</v>
+        <v>5.2299999999999995</v>
       </c>
       <c r="X13" s="54" t="s">
         <v>59</v>
@@ -2628,15 +2628,15 @@
       </c>
       <c r="O14" s="31">
         <f>IF(O8*$C$1/O9&lt;=10, O8*$C$1/O9, O8*$C$1/O9-10)</f>
-        <v>5.9358490566037743</v>
+        <v>5.825925925925926</v>
       </c>
       <c r="P14" s="52">
         <f>IF(O14&gt;1,VLOOKUP(O14*10,$AA$26:$AA$132,1)/10,IF(O14&gt;0.099,VLOOKUP(O14*100,$AB$26:$AB$132,1)/100,VLOOKUP(O14*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>5.9</v>
+        <v>5.76</v>
       </c>
       <c r="Q14" s="52">
         <f ca="1">IF(O14&gt;1,OFFSET($AA$26,MATCH(O14*10,$AA$26:$AA$132,1),0)/10,IF(O14&gt;0.099, OFFSET($AB$26,MATCH(O14*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O14*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>6.04</v>
+        <v>5.9</v>
       </c>
       <c r="R14" s="54" t="s">
         <v>59</v>
@@ -2723,15 +2723,15 @@
       </c>
       <c r="U15" s="31">
         <f>IF(U7-U9/U8*U7&gt;10, U7-U9/U8*U7-10, U7-U9/U8*U7)</f>
-        <v>2</v>
+        <v>7.8</v>
       </c>
       <c r="V15" s="52">
         <f>IF(U15&gt;1,VLOOKUP(U15*10,$AA$27:$AA$133,1)/10,IF(U15&gt;0.099,VLOOKUP(U15*100,$AB$27:$AB$133,1)/100,VLOOKUP(U15*1000,$AB$27:$AB$133,1)/1000))</f>
-        <v>2</v>
+        <v>7.68</v>
       </c>
       <c r="W15" s="52">
         <f ca="1">IF(U15&gt;1,OFFSET($AA$27,MATCH(U15*10,$AA$27:$AA$133,1),0)/10,IF(U15&gt;0.099, OFFSET($AB$27,MATCH(U15*100,$AB$27:$AB$133,1),0)/100,OFFSET($AB$27,MATCH(U15*1000,$AB$27:$AB$133,1),0)/1000))</f>
-        <v>2.0499999999999998</v>
+        <v>7.87</v>
       </c>
       <c r="X15" s="54" t="s">
         <v>59</v>
@@ -2776,15 +2776,15 @@
       </c>
       <c r="O16" s="31">
         <f>IF(O8*$C$1/O9&lt;=10, O8-O14, O8-O14-10)</f>
-        <v>7.0641509433962257</v>
+        <v>7.174074074074074</v>
       </c>
       <c r="P16" s="52">
         <f>IF(O16&gt;1,VLOOKUP(O16*10,$AA$26:$AA$132,1)/10,IF(O16&gt;0.099,VLOOKUP(O16*100,$AB$26:$AB$132,1)/100,VLOOKUP(O16*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>6.9799999999999995</v>
+        <v>7.15</v>
       </c>
       <c r="Q16" s="52">
         <f ca="1">IF(O16&gt;1,OFFSET($AA$26,MATCH(O16*10,$AA$26:$AA$132,1),0)/10,IF(O16&gt;0.099, OFFSET($AB$26,MATCH(O16*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O16*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>7.15</v>
+        <v>7.32</v>
       </c>
       <c r="R16" s="54" t="s">
         <v>59</v>
@@ -2794,15 +2794,15 @@
       </c>
       <c r="U16" s="31">
         <f>IF(U7-U9/U8*U7&lt;=10, 0, 10)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V16" s="52">
         <f>IF(U7-U9/U8*U7&lt;=10, 0, 10)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W16" s="52">
         <f>IF(U7-U9/U8*U7&lt;=10, 0, 10)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="X16" s="54" t="s">
         <v>59</v>
@@ -2838,11 +2838,11 @@
       <c r="O17" s="18"/>
       <c r="P17" s="53">
         <f>$C$1*(1+P16/(P14+P15))</f>
-        <v>2.6414915254237283</v>
+        <v>2.711996527777778</v>
       </c>
       <c r="Q17" s="53">
         <f ca="1">$C$1*(1+Q16/(Q14+Q15))</f>
-        <v>2.6423675496688741</v>
+        <v>2.7112203389830509</v>
       </c>
       <c r="R17" s="92" t="s">
         <v>1</v>
@@ -2853,11 +2853,11 @@
       <c r="U17" s="18"/>
       <c r="V17" s="53">
         <f>U8*(V13+V14)/(V13+V14+V15+V16)</f>
-        <v>0.39607448414695517</v>
+        <v>0.39953088350273658</v>
       </c>
       <c r="W17" s="53">
         <f ca="1">U8*(W13+W14)/(W13+W14+W15+W16)</f>
-        <v>0.40079562406762798</v>
+        <v>0.39923664122137403</v>
       </c>
       <c r="X17" s="54" t="s">
         <v>1</v>
@@ -2916,7 +2916,7 @@
         <v>45</v>
       </c>
       <c r="O19" s="13">
-        <v>5.9</v>
+        <v>5.76</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>58</v>
@@ -2927,7 +2927,7 @@
         <v>11</v>
       </c>
       <c r="U19" s="13">
-        <v>8.06</v>
+        <v>5.23</v>
       </c>
       <c r="V19" s="4" t="s">
         <v>58</v>
@@ -3010,7 +3010,7 @@
         <v>46</v>
       </c>
       <c r="O21" s="13">
-        <v>6.98</v>
+        <v>7.15</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>58</v>
@@ -3021,7 +3021,7 @@
         <v>12</v>
       </c>
       <c r="U21" s="13">
-        <v>2</v>
+        <v>7.87</v>
       </c>
       <c r="V21" s="4" t="s">
         <v>58</v>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="U22" s="31">
         <f>U16</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V22" s="4" t="s">
         <v>58</v>
@@ -3102,11 +3102,11 @@
       </c>
       <c r="O23" s="64">
         <f>$C$1*(1+O21/(O19+O20))</f>
-        <v>2.6414915254237292</v>
+        <v>2.711996527777778</v>
       </c>
       <c r="P23" s="65">
         <f>(O23-O9)/O23*100</f>
-        <v>-0.32210872131818852</v>
+        <v>0.44235041066250291</v>
       </c>
       <c r="Q23" s="94" t="s">
         <v>2</v>
@@ -3154,14 +3154,14 @@
       </c>
       <c r="U24" s="67">
         <f>U8*(U19+U20)/(U19+U20+U21+U22)</f>
-        <v>0.40179461615154533</v>
+        <v>0.39923664122137403</v>
       </c>
       <c r="V24" s="80" t="s">
         <v>1</v>
       </c>
       <c r="W24" s="81">
         <f>(U24-U9)/U24*100</f>
-        <v>0.44665012406946381</v>
+        <v>-0.1912045889101425</v>
       </c>
       <c r="X24" s="82" t="s">
         <v>2</v>

</xml_diff>